<commit_message>
Se actualiza el proyecto (diagrama de requisitos, analisis, y colaboracion)
</commit_message>
<xml_diff>
--- a/Documentacion/Descripcion- Casos de Requisitos.xlsx
+++ b/Documentacion/Descripcion- Casos de Requisitos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="180" windowWidth="15480" windowHeight="8385"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="105">
   <si>
     <t>Actores</t>
   </si>
@@ -309,13 +309,46 @@
   <si>
     <t>1) Ingresar datos del destinatario.(razón o nombre y apellido, dirección,  teléfono)
 2) Ingresa datos del paquete. (numero o código de etiqueta)</t>
+  </si>
+  <si>
+    <t>Caso de Usos de Requisitos</t>
+  </si>
+  <si>
+    <t>Registrar Zonas</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Administrador- Registrar Zonas: Relacion de Asociación</t>
+  </si>
+  <si>
+    <t>Proposito</t>
+  </si>
+  <si>
+    <t>Registra todas las zonas de reparto que abarca la empresa a nivel nacional y extranjero</t>
+  </si>
+  <si>
+    <t>Registrar Zonas de Reparto</t>
+  </si>
+  <si>
+    <t>El sistema debe tener cargados las ciudades, provincias y paises</t>
+  </si>
+  <si>
+    <t>1) Ingresar Nombre de la zona, Ciudadad, y la descripcion (desde donde hasta donde abarca)</t>
+  </si>
+  <si>
+    <t>2) Guardar</t>
+  </si>
+  <si>
+    <t>No existe la ciudad, provincia ni pais de esa Zona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,7 +575,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -577,7 +609,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -753,20 +784,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:XFC133"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:XFC146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B113" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136:B146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="78.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
@@ -774,7 +805,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="18" t="s">
         <v>43</v>
       </c>
@@ -782,7 +813,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -790,7 +821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
@@ -798,7 +829,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="17" t="s">
         <v>41</v>
       </c>
@@ -806,7 +837,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
@@ -814,7 +845,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
@@ -822,7 +853,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="45">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
@@ -830,7 +861,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="30">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -838,13 +869,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="4"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -852,7 +883,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="18" t="s">
         <v>43</v>
       </c>
@@ -860,7 +891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>0</v>
       </c>
@@ -868,7 +899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" s="13" t="s">
         <v>1</v>
       </c>
@@ -876,7 +907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="17" t="s">
         <v>41</v>
       </c>
@@ -884,7 +915,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
         <v>2</v>
       </c>
@@ -892,7 +923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
         <v>3</v>
       </c>
@@ -900,7 +931,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="30">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -908,13 +939,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="30">
       <c r="A24" s="5" t="s">
         <v>6</v>
       </c>
@@ -922,11 +953,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="10"/>
       <c r="B25" s="8"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="9" t="s">
         <v>7</v>
       </c>
@@ -934,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="18" t="s">
         <v>43</v>
       </c>
@@ -942,7 +973,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
         <v>0</v>
       </c>
@@ -950,7 +981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="13" t="s">
         <v>1</v>
       </c>
@@ -958,7 +989,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="6" t="s">
         <v>41</v>
       </c>
@@ -966,7 +997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>2</v>
       </c>
@@ -974,7 +1005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>3</v>
       </c>
@@ -982,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="63" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>4</v>
       </c>
@@ -990,7 +1021,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
@@ -998,7 +1029,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="15.75" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="9" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1045,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="18" t="s">
         <v>43</v>
       </c>
@@ -1022,7 +1053,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -1030,7 +1061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="17" t="s">
         <v>1</v>
       </c>
@@ -1038,7 +1069,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="17" t="s">
         <v>41</v>
       </c>
@@ -1046,7 +1077,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="5" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1085,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="5" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1093,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="30">
       <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
@@ -1070,7 +1101,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="5" t="s">
         <v>5</v>
       </c>
@@ -1078,13 +1109,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B49" s="4"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="9" t="s">
         <v>7</v>
       </c>
@@ -1092,7 +1123,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="18" t="s">
         <v>43</v>
       </c>
@@ -1100,7 +1131,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="5" t="s">
         <v>0</v>
       </c>
@@ -1108,7 +1139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="17" t="s">
         <v>1</v>
       </c>
@@ -1116,7 +1147,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="17" t="s">
         <v>41</v>
       </c>
@@ -1124,7 +1155,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="5" t="s">
         <v>2</v>
       </c>
@@ -1132,7 +1163,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="5" t="s">
         <v>3</v>
       </c>
@@ -1140,7 +1171,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="75">
       <c r="A59" s="5" t="s">
         <v>4</v>
       </c>
@@ -1148,19 +1179,19 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="4"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B61" s="4"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="9" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="18" t="s">
         <v>43</v>
       </c>
@@ -1176,7 +1207,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="6" t="s">
         <v>1</v>
       </c>
@@ -1192,7 +1223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="6" t="s">
         <v>41</v>
       </c>
@@ -1200,7 +1231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="5" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1239,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="5" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1247,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="30">
       <c r="A71" s="5" t="s">
         <v>4</v>
       </c>
@@ -1224,13 +1255,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B72" s="4"/>
     </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="30">
       <c r="A73" s="5" t="s">
         <v>6</v>
       </c>
@@ -1238,15 +1269,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="10"/>
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" s="14" customFormat="1">
       <c r="A75" s="10"/>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" s="14" customFormat="1">
       <c r="A76" s="9" t="s">
         <v>7</v>
       </c>
@@ -1254,7 +1285,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" s="14" customFormat="1">
       <c r="A77" s="18" t="s">
         <v>43</v>
       </c>
@@ -1262,7 +1293,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="78" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" s="14" customFormat="1">
       <c r="A78" s="5" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1301,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" s="14" customFormat="1">
       <c r="A79" s="6" t="s">
         <v>1</v>
       </c>
@@ -1278,7 +1309,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" s="14" customFormat="1">
       <c r="A80" s="6" t="s">
         <v>41</v>
       </c>
@@ -1286,7 +1317,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" s="14" customFormat="1">
       <c r="A81" s="5" t="s">
         <v>2</v>
       </c>
@@ -1294,7 +1325,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" s="14" customFormat="1">
       <c r="A82" s="5" t="s">
         <v>3</v>
       </c>
@@ -1302,7 +1333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="45">
       <c r="A83" s="5" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="5" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1349,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="5" t="s">
         <v>6</v>
       </c>
@@ -1326,15 +1357,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="10"/>
       <c r="B86" s="3"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="10"/>
       <c r="B87" s="3"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" s="9" t="s">
         <v>7</v>
       </c>
@@ -1342,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="18" t="s">
         <v>43</v>
       </c>
@@ -1350,7 +1381,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="5" t="s">
         <v>0</v>
       </c>
@@ -1358,7 +1389,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="30">
       <c r="A92" s="6" t="s">
         <v>1</v>
       </c>
@@ -1366,7 +1397,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" s="6" t="s">
         <v>41</v>
       </c>
@@ -1374,7 +1405,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="11" t="s">
         <v>2</v>
       </c>
@@ -1382,7 +1413,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="5" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1421,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="11" t="s">
         <v>4</v>
       </c>
@@ -1398,13 +1429,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="5" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1443,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" s="9" t="s">
         <v>7</v>
       </c>
@@ -1420,7 +1451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="18" t="s">
         <v>43</v>
       </c>
@@ -1428,7 +1459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" s="5" t="s">
         <v>0</v>
       </c>
@@ -1436,7 +1467,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="30">
       <c r="A104" s="6" t="s">
         <v>1</v>
       </c>
@@ -1444,7 +1475,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" s="6" t="s">
         <v>41</v>
       </c>
@@ -1452,7 +1483,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" s="11" t="s">
         <v>2</v>
       </c>
@@ -1460,7 +1491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2">
       <c r="A107" s="5" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1499,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2">
       <c r="A108" s="15" t="s">
         <v>4</v>
       </c>
@@ -1476,19 +1507,19 @@
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2">
       <c r="A109" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B109" s="2"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2">
       <c r="A110" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B110" s="2"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2">
       <c r="A112" s="9" t="s">
         <v>7</v>
       </c>
@@ -1496,7 +1527,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A113" s="18" t="s">
         <v>43</v>
       </c>
@@ -1504,7 +1535,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="114" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A114" s="5" t="s">
         <v>0</v>
       </c>
@@ -1512,7 +1543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A115" s="6" t="s">
         <v>1</v>
       </c>
@@ -1520,7 +1551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="116" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A116" s="6" t="s">
         <v>41</v>
       </c>
@@ -1528,7 +1559,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="117" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A117" s="11" t="s">
         <v>2</v>
       </c>
@@ -1536,7 +1567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="118" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A118" s="5" t="s">
         <v>3</v>
       </c>
@@ -1544,7 +1575,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A119" s="7" t="s">
         <v>4</v>
       </c>
@@ -1552,7 +1583,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="45">
       <c r="A120" s="5" t="s">
         <v>5</v>
       </c>
@@ -1560,7 +1591,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="121" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A121" s="5" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1599,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="124" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A124" s="9" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +1607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A125" s="18" t="s">
         <v>43</v>
       </c>
@@ -1584,7 +1615,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="126" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A126" s="5" t="s">
         <v>0</v>
       </c>
@@ -1592,7 +1623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="127" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383">
       <c r="A127" s="6" t="s">
         <v>1</v>
       </c>
@@ -1600,7 +1631,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="128" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" s="3" customFormat="1">
       <c r="A128" s="6" t="s">
         <v>41</v>
       </c>
@@ -9799,7 +9830,7 @@
       <c r="XFA128" s="10"/>
       <c r="XFC128" s="10"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2">
       <c r="A129" s="11" t="s">
         <v>2</v>
       </c>
@@ -9807,7 +9838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2">
       <c r="A130" s="19" t="s">
         <v>3</v>
       </c>
@@ -9815,7 +9846,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2">
       <c r="A131" s="7" t="s">
         <v>4</v>
       </c>
@@ -9823,17 +9854,101 @@
         <v>25</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2">
       <c r="A132" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2">
       <c r="A133" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B133" s="2"/>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="5"/>
+      <c r="B144" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B145" s="2"/>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9842,24 +9957,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>